<commit_message>
updated ocean realm model and change the status of publishing
</commit_message>
<xml_diff>
--- a/cmip6/models/iitm-esm/cmip6_cccr-iitm_iitm-esm_ocean.xlsx
+++ b/cmip6/models/iitm-esm/cmip6_cccr-iitm_iitm-esm_ocean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2745" yWindow="-150" windowWidth="16095" windowHeight="9660" tabRatio="865" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="8. Uplow Boundaries" sheetId="9" r:id="rId9"/>
     <sheet name="9. Boundary Forcing" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="871">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -2607,6 +2607,39 @@
   </si>
   <si>
     <t>cmip6.ocean.boundary_forcing.tracers.fresh_water_forcing.forced_mode_restoring</t>
+  </si>
+  <si>
+    <t>Tfreeze=0.054*salinity</t>
+  </si>
+  <si>
+    <t>Tripolar grid  varing  resolution (0.33 degrees between -10 to 10) reduces poleward to 1 degree</t>
+  </si>
+  <si>
+    <t>Tripolar grid</t>
+  </si>
+  <si>
+    <t>2nd ordered centered</t>
+  </si>
+  <si>
+    <t>Skew Flux</t>
+  </si>
+  <si>
+    <t>Flow Dependent</t>
+  </si>
+  <si>
+    <t>Barotrophic &amp; Baroclinic tides</t>
+  </si>
+  <si>
+    <t>Turbulance Closure (KPP)</t>
+  </si>
+  <si>
+    <t>Turbulent closure (KPP)</t>
+  </si>
+  <si>
+    <t>via sea ice</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -3081,9 +3114,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3092,12 +3125,12 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3105,7 +3138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="23.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3113,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="23.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3121,7 +3154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="23.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -3129,7 +3162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -3137,47 +3170,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="23.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="23.25">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="23.25">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="23.25">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="23.25">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="23.25">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="23.25">
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="23.25">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="23.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -3185,7 +3218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="23.25">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -3193,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="23.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -3212,9 +3245,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD110"/>
+  <dimension ref="A1:AF110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3283,7 +3318,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
@@ -3306,7 +3341,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>869</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="7" t="s">
@@ -3332,8 +3369,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="178" customHeight="1">
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B20" s="11" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="7" t="s">
@@ -3359,8 +3398,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="24" customHeight="1">
       <c r="A27" s="7" t="s">
@@ -3386,7 +3427,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="178" customHeight="1">
+    <row r="30" spans="1:3" ht="177.95" customHeight="1">
       <c r="B30" s="11"/>
     </row>
     <row r="32" spans="1:3" ht="24" customHeight="1">
@@ -3413,7 +3454,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="178" customHeight="1">
+    <row r="35" spans="1:3" ht="177.95" customHeight="1">
       <c r="B35" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
@@ -3440,7 +3481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="178" customHeight="1">
+    <row r="40" spans="1:3" ht="177.95" customHeight="1">
       <c r="B40" s="11"/>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
@@ -3511,7 +3552,9 @@
       </c>
     </row>
     <row r="56" spans="1:32" ht="24" customHeight="1">
-      <c r="B56" s="11"/>
+      <c r="B56" s="11" t="s">
+        <v>804</v>
+      </c>
       <c r="AA56" s="5" t="s">
         <v>86</v>
       </c>
@@ -3564,7 +3607,9 @@
       </c>
     </row>
     <row r="64" spans="1:32" ht="24" customHeight="1">
-      <c r="B64" s="11"/>
+      <c r="B64" s="11" t="s">
+        <v>814</v>
+      </c>
       <c r="AA64" s="5" t="s">
         <v>333</v>
       </c>
@@ -3646,7 +3691,9 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="24" customHeight="1">
-      <c r="B80" s="11"/>
+      <c r="B80" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="AA80" s="5" t="s">
         <v>827</v>
       </c>
@@ -3680,7 +3727,9 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="24" customHeight="1">
-      <c r="B84" s="11"/>
+      <c r="B84" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="24" customHeight="1">
       <c r="A86" s="7" t="s">
@@ -3706,7 +3755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="178" customHeight="1">
+    <row r="89" spans="1:3" ht="177.95" customHeight="1">
       <c r="B89" s="11"/>
     </row>
     <row r="91" spans="1:3" ht="24" customHeight="1">
@@ -3863,7 +3912,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3874,7 +3923,7 @@
     <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -3882,7 +3931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
@@ -3890,7 +3939,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
@@ -3903,10 +3952,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="18">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="18">
       <c r="A8" s="7" t="s">
         <v>32</v>
       </c>
@@ -3914,7 +3963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
@@ -3927,7 +3976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
@@ -3937,9 +3986,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD210"/>
+  <dimension ref="A1:AH214"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B217" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4035,7 +4086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
       <c r="B16" s="11"/>
     </row>
     <row r="18" spans="1:34" ht="24" customHeight="1">
@@ -4058,7 +4109,9 @@
       </c>
     </row>
     <row r="20" spans="1:34" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="AA20" s="5" t="s">
         <v>57</v>
       </c>
@@ -4097,7 +4150,9 @@
       </c>
     </row>
     <row r="25" spans="1:34" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="AA25" s="5" t="s">
         <v>65</v>
       </c>
@@ -4108,6 +4163,23 @@
         <v>67</v>
       </c>
       <c r="AD25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="18">
+      <c r="B26" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD26" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4136,7 +4208,9 @@
       </c>
     </row>
     <row r="30" spans="1:34" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
+      <c r="B30" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="AA30" s="5" t="s">
         <v>72</v>
       </c>
@@ -4162,121 +4236,269 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="24" customHeight="1">
-      <c r="A33" s="12" t="s">
+    <row r="31" spans="1:34" ht="24" customHeight="1">
+      <c r="B31" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF31" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH31" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" ht="24" customHeight="1">
+      <c r="B32" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC32" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH32" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" ht="24" customHeight="1">
+      <c r="B33" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF33" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH33" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="24" customHeight="1">
+      <c r="B34" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC34" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF34" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG34" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" ht="24" customHeight="1">
+      <c r="B35" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC35" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD35" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG35" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH35" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="24" customHeight="1">
+      <c r="B36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF36" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG36" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" ht="24" customHeight="1">
+      <c r="A37" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B37" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="24" customHeight="1">
-      <c r="B34" s="13" t="s">
+    <row r="38" spans="1:34" ht="24" customHeight="1">
+      <c r="B38" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="24" customHeight="1">
-      <c r="A36" s="7" t="s">
+    <row r="40" spans="1:34" ht="24" customHeight="1">
+      <c r="A40" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="24" customHeight="1">
-      <c r="A37" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:32" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
-      <c r="AA38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB38" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC38" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD38" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE38" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF38" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32" ht="24" customHeight="1">
-      <c r="A40" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" ht="24" customHeight="1">
+    <row r="41" spans="1:34" ht="24" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32" ht="24" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="24" customHeight="1">
       <c r="B42" s="11"/>
       <c r="AA42" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="AB42" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32" ht="24" customHeight="1">
+        <v>87</v>
+      </c>
+      <c r="AC42" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF42" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="24" customHeight="1">
       <c r="A44" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" ht="24" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" ht="24" customHeight="1">
       <c r="A45" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32" ht="24" customHeight="1">
-      <c r="B46" s="11"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" ht="24" customHeight="1">
+      <c r="B46" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="AA46" s="5" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="AB46" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32" ht="24" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" ht="24" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="24" customHeight="1">
@@ -4284,27 +4506,29 @@
         <v>54</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="24" customHeight="1">
-      <c r="B50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>99</v>
+      </c>
       <c r="AA50" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="AB50" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="24" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="24" customHeight="1">
@@ -4312,49 +4536,62 @@
         <v>54</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="24" customHeight="1">
-      <c r="B54" s="11"/>
+      <c r="B54" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="AA54" s="5" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="AB54" s="5" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="24" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="24" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="24" customHeight="1">
-      <c r="B58" s="11"/>
+      <c r="B58" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="AA58" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB58" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="60" spans="1:28" ht="24" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="24" customHeight="1">
@@ -4362,247 +4599,253 @@
         <v>113</v>
       </c>
       <c r="B61" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" ht="24" customHeight="1">
+      <c r="B62" s="11">
+        <v>3992.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="24" customHeight="1">
+      <c r="A64" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:32" ht="24" customHeight="1">
+      <c r="A65" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
-    </row>
-    <row r="65" spans="1:32" ht="24" customHeight="1">
-      <c r="A65" s="12" t="s">
+    <row r="66" spans="1:32" ht="24" customHeight="1">
+      <c r="B66" s="11"/>
+    </row>
+    <row r="69" spans="1:32" ht="24" customHeight="1">
+      <c r="A69" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B69" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:32" ht="24" customHeight="1">
-      <c r="B66" s="13" t="s">
+    <row r="70" spans="1:32" ht="24" customHeight="1">
+      <c r="B70" s="13" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="68" spans="1:32" ht="24" customHeight="1">
-      <c r="A68" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:32" ht="24" customHeight="1">
-      <c r="A69" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="1:32" ht="24" customHeight="1">
-      <c r="B70" s="11"/>
-      <c r="AA70" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB70" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC70" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD70" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE70" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF70" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="24" customHeight="1">
       <c r="A72" s="7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:32" ht="24" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>134</v>
+        <v>54</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:32" ht="24" customHeight="1">
-      <c r="B74" s="11"/>
+      <c r="B74" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA74" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB74" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC74" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD74" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE74" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF74" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="76" spans="1:32" ht="24" customHeight="1">
       <c r="A76" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:32" ht="24" customHeight="1">
       <c r="A77" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" ht="24" customHeight="1">
+      <c r="B78" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32" ht="24" customHeight="1">
+      <c r="A80" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="24" customHeight="1">
+      <c r="A81" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B81" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C81" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="1:32" ht="24" customHeight="1">
-      <c r="B78" s="10" t="s">
+    <row r="82" spans="1:3" ht="24" customHeight="1">
+      <c r="B82" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="79" spans="1:32" ht="178" customHeight="1">
-      <c r="B79" s="11"/>
-    </row>
-    <row r="81" spans="1:3" ht="24" customHeight="1">
-      <c r="A81" s="7" t="s">
+    <row r="83" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B83" s="11"/>
+    </row>
+    <row r="85" spans="1:3" ht="24" customHeight="1">
+      <c r="A85" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="24" customHeight="1">
-      <c r="A82" s="8" t="s">
+    <row r="86" spans="1:3" ht="24" customHeight="1">
+      <c r="A86" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B86" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C86" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24" customHeight="1">
-      <c r="B83" s="11"/>
-    </row>
-    <row r="86" spans="1:3" ht="24" customHeight="1">
-      <c r="A86" s="12" t="s">
+    <row r="87" spans="1:3" ht="24" customHeight="1">
+      <c r="B87" s="11"/>
+    </row>
+    <row r="90" spans="1:3" ht="24" customHeight="1">
+      <c r="A90" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B90" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="24" customHeight="1">
-      <c r="B87" s="13" t="s">
+    <row r="91" spans="1:3" ht="24" customHeight="1">
+      <c r="B91" s="13" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="24" customHeight="1">
-      <c r="A89" s="7" t="s">
+    <row r="93" spans="1:3" ht="24" customHeight="1">
+      <c r="A93" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="24" customHeight="1">
-      <c r="A90" s="8" t="s">
+    <row r="94" spans="1:3" ht="24" customHeight="1">
+      <c r="A94" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B94" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C94" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="24" customHeight="1">
-      <c r="B91" s="10" t="s">
+    <row r="95" spans="1:3" ht="24" customHeight="1">
+      <c r="B95" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="178" customHeight="1">
-      <c r="B92" s="11"/>
-    </row>
-    <row r="94" spans="1:3" ht="24" customHeight="1">
-      <c r="A94" s="7" t="s">
+    <row r="96" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B96" s="11"/>
+    </row>
+    <row r="98" spans="1:3" ht="24" customHeight="1">
+      <c r="A98" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B98" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="24" customHeight="1">
-      <c r="A95" s="8" t="s">
+    <row r="99" spans="1:3" ht="24" customHeight="1">
+      <c r="A99" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C99" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24" customHeight="1">
-      <c r="B96" s="10" t="s">
+    <row r="100" spans="1:3" ht="24" customHeight="1">
+      <c r="B100" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="178" customHeight="1">
-      <c r="B97" s="11"/>
-    </row>
-    <row r="100" spans="1:3" ht="24" customHeight="1">
-      <c r="A100" s="12" t="s">
+    <row r="101" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B101" s="11"/>
+    </row>
+    <row r="104" spans="1:3" ht="24" customHeight="1">
+      <c r="A104" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B104" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24" customHeight="1">
-      <c r="B101" s="13" t="s">
+    <row r="105" spans="1:3" ht="24" customHeight="1">
+      <c r="B105" s="13" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
-      <c r="A103" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
-      <c r="A104" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1">
       <c r="A107" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="24" customHeight="1">
@@ -4610,10 +4853,10 @@
         <v>29</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="24" customHeight="1">
@@ -4621,10 +4864,10 @@
     </row>
     <row r="111" spans="1:3" ht="24" customHeight="1">
       <c r="A111" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
@@ -4632,61 +4875,61 @@
         <v>29</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="24" customHeight="1">
+      <c r="B113" s="11"/>
+    </row>
+    <row r="115" spans="1:3" ht="24" customHeight="1">
+      <c r="A115" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="24" customHeight="1">
+      <c r="A116" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B116" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C116" s="9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24" customHeight="1">
-      <c r="B113" s="10" t="s">
+    <row r="117" spans="1:3" ht="24" customHeight="1">
+      <c r="B117" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="24" customHeight="1">
-      <c r="B114" s="11"/>
-    </row>
-    <row r="117" spans="1:3" ht="24" customHeight="1">
-      <c r="A117" s="12" t="s">
+    <row r="118" spans="1:3" ht="24" customHeight="1">
+      <c r="B118" s="11"/>
+    </row>
+    <row r="121" spans="1:3" ht="24" customHeight="1">
+      <c r="A121" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B117" s="12" t="s">
+      <c r="B121" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="24" customHeight="1">
-      <c r="B118" s="13" t="s">
+    <row r="122" spans="1:3" ht="24" customHeight="1">
+      <c r="B122" s="13" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="24" customHeight="1">
-      <c r="A120" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B120" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="24" customHeight="1">
-      <c r="A121" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B121" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="24" customHeight="1">
-      <c r="B122" s="11"/>
     </row>
     <row r="124" spans="1:3" ht="24" customHeight="1">
       <c r="A124" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="24" customHeight="1">
@@ -4694,10 +4937,10 @@
         <v>29</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1">
@@ -4705,10 +4948,10 @@
     </row>
     <row r="128" spans="1:3" ht="24" customHeight="1">
       <c r="A128" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
@@ -4716,10 +4959,10 @@
         <v>29</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
@@ -4727,10 +4970,10 @@
     </row>
     <row r="132" spans="1:3" ht="24" customHeight="1">
       <c r="A132" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="24" customHeight="1">
@@ -4738,32 +4981,34 @@
         <v>29</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
-      <c r="B134" s="11"/>
+      <c r="B134" s="11" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="136" spans="1:3" ht="24" customHeight="1">
       <c r="A136" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="8" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
@@ -4771,10 +5016,10 @@
     </row>
     <row r="140" spans="1:3" ht="24" customHeight="1">
       <c r="A140" s="7" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="24" customHeight="1">
@@ -4782,100 +5027,108 @@
         <v>190</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="24" customHeight="1">
-      <c r="B142" s="11"/>
+      <c r="B142" s="11">
+        <v>72000</v>
+      </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
       <c r="A144" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="24" customHeight="1">
       <c r="A145" s="8" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
-      <c r="B146" s="11"/>
+      <c r="B146" s="11">
+        <v>50</v>
+      </c>
     </row>
     <row r="148" spans="1:3" ht="24" customHeight="1">
       <c r="A148" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
       <c r="A149" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="24" customHeight="1">
+      <c r="B150" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="24" customHeight="1">
+      <c r="A152" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="24" customHeight="1">
+      <c r="A153" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B149" s="9" t="s">
+      <c r="B153" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C149" s="9" t="s">
+      <c r="C153" s="9" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="24" customHeight="1">
-      <c r="B150" s="11"/>
-    </row>
-    <row r="153" spans="1:3" ht="24" customHeight="1">
-      <c r="A153" s="12" t="s">
+    <row r="154" spans="1:3" ht="24" customHeight="1">
+      <c r="B154" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="24" customHeight="1">
+      <c r="A157" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="B153" s="12" t="s">
+      <c r="B157" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="24" customHeight="1">
-      <c r="B154" s="13" t="s">
+    <row r="158" spans="1:3" ht="24" customHeight="1">
+      <c r="B158" s="13" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" ht="24" customHeight="1">
-      <c r="A156" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="24" customHeight="1">
-      <c r="A157" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B157" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C157" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="24" customHeight="1">
-      <c r="B158" s="11"/>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
       <c r="A160" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>212</v>
+        <v>48</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
@@ -4883,142 +5136,142 @@
         <v>29</v>
       </c>
       <c r="B161" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="24" customHeight="1">
+      <c r="B162" s="11"/>
+    </row>
+    <row r="164" spans="1:3" ht="24" customHeight="1">
+      <c r="A164" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="24" customHeight="1">
+      <c r="A165" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B165" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C161" s="9" t="s">
+      <c r="C165" s="9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="24" customHeight="1">
-      <c r="B162" s="10" t="s">
+    <row r="166" spans="1:3" ht="24" customHeight="1">
+      <c r="B166" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="178" customHeight="1">
-      <c r="B163" s="11"/>
-    </row>
-    <row r="165" spans="1:3" ht="24" customHeight="1">
-      <c r="A165" s="7" t="s">
+    <row r="167" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B167" s="11"/>
+    </row>
+    <row r="169" spans="1:3" ht="24" customHeight="1">
+      <c r="A169" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B169" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="24" customHeight="1">
-      <c r="A166" s="8" t="s">
+    <row r="170" spans="1:3" ht="24" customHeight="1">
+      <c r="A170" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B166" s="9" t="s">
+      <c r="B170" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C166" s="9" t="s">
+      <c r="C170" s="9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="24" customHeight="1">
-      <c r="B167" s="10" t="s">
+    <row r="171" spans="1:3" ht="24" customHeight="1">
+      <c r="B171" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="24" customHeight="1">
-      <c r="B168" s="11"/>
-    </row>
-    <row r="170" spans="1:3" ht="24" customHeight="1">
-      <c r="A170" s="7" t="s">
+    <row r="172" spans="1:3" ht="24" customHeight="1">
+      <c r="B172" s="11"/>
+    </row>
+    <row r="174" spans="1:3" ht="24" customHeight="1">
+      <c r="A174" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B170" s="7" t="s">
+      <c r="B174" s="7" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="24" customHeight="1">
-      <c r="A171" s="8" t="s">
+    <row r="175" spans="1:3" ht="24" customHeight="1">
+      <c r="A175" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B171" s="9" t="s">
+      <c r="B175" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C171" s="9" t="s">
+      <c r="C175" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="24" customHeight="1">
-      <c r="B172" s="10" t="s">
+    <row r="176" spans="1:3" ht="24" customHeight="1">
+      <c r="B176" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="24" customHeight="1">
-      <c r="B173" s="11"/>
-    </row>
-    <row r="175" spans="1:3" ht="24" customHeight="1">
-      <c r="A175" s="7" t="s">
+    <row r="177" spans="1:3" ht="24" customHeight="1">
+      <c r="B177" s="11"/>
+    </row>
+    <row r="179" spans="1:3" ht="24" customHeight="1">
+      <c r="A179" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B175" s="7" t="s">
+      <c r="B179" s="7" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="24" customHeight="1">
-      <c r="A176" s="8" t="s">
+    <row r="180" spans="1:3" ht="24" customHeight="1">
+      <c r="A180" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B176" s="9" t="s">
+      <c r="B180" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C176" s="9" t="s">
+      <c r="C180" s="9" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="24" customHeight="1">
-      <c r="B177" s="10" t="s">
+    <row r="181" spans="1:3" ht="24" customHeight="1">
+      <c r="B181" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="24" customHeight="1">
-      <c r="B178" s="11"/>
-    </row>
-    <row r="181" spans="1:3" ht="24" customHeight="1">
-      <c r="A181" s="12" t="s">
+    <row r="182" spans="1:3" ht="24" customHeight="1">
+      <c r="B182" s="11"/>
+    </row>
+    <row r="185" spans="1:3" ht="24" customHeight="1">
+      <c r="A185" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="B181" s="12" t="s">
+      <c r="B185" s="12" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="24" customHeight="1">
-      <c r="B182" s="13" t="s">
+    <row r="186" spans="1:3" ht="24" customHeight="1">
+      <c r="B186" s="13" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" ht="24" customHeight="1">
-      <c r="A184" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="24" customHeight="1">
-      <c r="A185" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B185" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C185" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="24" customHeight="1">
-      <c r="B186" s="11"/>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
       <c r="A188" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>212</v>
+        <v>48</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
@@ -5026,199 +5279,186 @@
         <v>29</v>
       </c>
       <c r="B189" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="24" customHeight="1">
+      <c r="B190" s="11"/>
+    </row>
+    <row r="192" spans="1:3" ht="24" customHeight="1">
+      <c r="A192" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="193" spans="1:32" ht="24" customHeight="1">
+      <c r="A193" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B193" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C189" s="9" t="s">
+      <c r="C193" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="24" customHeight="1">
-      <c r="B190" s="10" t="s">
+    <row r="194" spans="1:32" ht="24" customHeight="1">
+      <c r="B194" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="178" customHeight="1">
-      <c r="B191" s="11"/>
-    </row>
-    <row r="193" spans="1:32" ht="24" customHeight="1">
-      <c r="A193" s="7" t="s">
+    <row r="195" spans="1:32" ht="177.95" customHeight="1">
+      <c r="B195" s="11"/>
+    </row>
+    <row r="197" spans="1:32" ht="24" customHeight="1">
+      <c r="A197" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="B193" s="7" t="s">
+      <c r="B197" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="194" spans="1:32" ht="24" customHeight="1">
-      <c r="A194" s="8" t="s">
+    <row r="198" spans="1:32" ht="24" customHeight="1">
+      <c r="A198" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B194" s="9" t="s">
+      <c r="B198" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C194" s="9" t="s">
+      <c r="C198" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="195" spans="1:32" ht="24" customHeight="1">
-      <c r="B195" s="10" t="s">
+    <row r="199" spans="1:32" ht="24" customHeight="1">
+      <c r="B199" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="196" spans="1:32" ht="24" customHeight="1">
-      <c r="B196" s="11"/>
-      <c r="AA196" s="5" t="s">
+    <row r="200" spans="1:32" ht="24" customHeight="1">
+      <c r="B200" s="11"/>
+      <c r="AA200" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="AB196" s="5" t="s">
+      <c r="AB200" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="AC196" s="5" t="s">
+      <c r="AC200" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="AD196" s="5" t="s">
+      <c r="AD200" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="AE196" s="5" t="s">
+      <c r="AE200" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="AF196" s="5" t="s">
+      <c r="AF200" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="198" spans="1:32" ht="24" customHeight="1">
-      <c r="A198" s="7" t="s">
+    <row r="202" spans="1:32" ht="24" customHeight="1">
+      <c r="A202" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="B198" s="7" t="s">
+      <c r="B202" s="7" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="199" spans="1:32" ht="24" customHeight="1">
-      <c r="A199" s="8" t="s">
+    <row r="203" spans="1:32" ht="24" customHeight="1">
+      <c r="A203" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B199" s="9" t="s">
+      <c r="B203" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="C199" s="9" t="s">
+      <c r="C203" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="200" spans="1:32" ht="24" customHeight="1">
-      <c r="B200" s="10" t="s">
+    <row r="204" spans="1:32" ht="24" customHeight="1">
+      <c r="B204" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="201" spans="1:32" ht="24" customHeight="1">
-      <c r="B201" s="11"/>
-    </row>
-    <row r="203" spans="1:32" ht="24" customHeight="1">
-      <c r="A203" s="7" t="s">
+    <row r="205" spans="1:32" ht="24" customHeight="1">
+      <c r="B205" s="11"/>
+    </row>
+    <row r="207" spans="1:32" ht="24" customHeight="1">
+      <c r="A207" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B203" s="7" t="s">
+      <c r="B207" s="7" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="204" spans="1:32" ht="24" customHeight="1">
-      <c r="A204" s="8" t="s">
+    <row r="208" spans="1:32" ht="24" customHeight="1">
+      <c r="A208" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B204" s="9" t="s">
+      <c r="B208" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="C204" s="9" t="s">
+      <c r="C208" s="9" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="205" spans="1:32" ht="24" customHeight="1">
-      <c r="B205" s="10" t="s">
+    <row r="209" spans="1:3" ht="24" customHeight="1">
+      <c r="B209" s="10" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="206" spans="1:32" ht="24" customHeight="1">
-      <c r="B206" s="11"/>
-    </row>
-    <row r="208" spans="1:32" ht="24" customHeight="1">
-      <c r="A208" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B208" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="24" customHeight="1">
-      <c r="A209" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B209" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C209" s="9" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="24" customHeight="1">
       <c r="B210" s="11"/>
     </row>
+    <row r="212" spans="1:3" ht="24" customHeight="1">
+      <c r="A212" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B212" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="24" customHeight="1">
+      <c r="A213" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="24" customHeight="1">
+      <c r="B214" s="11"/>
+    </row>
   </sheetData>
-  <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B25:B26">
       <formula1>AA20:AD20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
-      <formula1>AA25:AD25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:B36">
       <formula1>AA30:AH30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
-      <formula1>AA38:AF38</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42 B200 B74">
+      <formula1>AA42:AF42</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
-      <formula1>AA42:AB42</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46 B58 B54 B50">
       <formula1>AA46:AB46</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50">
-      <formula1>AA50:AB50</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62 B154 B66">
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54">
-      <formula1>AA54:AB54</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B58">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70">
-      <formula1>AA70:AF70</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78 B214 B150">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B138">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B142 B146">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B142">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B146">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B150">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B196">
-      <formula1>AA196:AF196</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B210">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5227,9 +5467,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD47"/>
+  <dimension ref="A1:AN47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B38" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5298,7 +5540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -5369,7 +5611,9 @@
       </c>
     </row>
     <row r="27" spans="1:40" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>279</v>
+      </c>
       <c r="AA27" s="5" t="s">
         <v>279</v>
       </c>
@@ -5433,7 +5677,9 @@
       </c>
     </row>
     <row r="31" spans="1:40" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:31" ht="24" customHeight="1">
       <c r="A34" s="12" t="s">
@@ -5468,7 +5714,12 @@
       </c>
     </row>
     <row r="39" spans="1:31" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>862</v>
+      </c>
       <c r="AA39" s="5" t="s">
         <v>302</v>
       </c>
@@ -5539,7 +5790,9 @@
       </c>
     </row>
     <row r="47" spans="1:31" ht="24" customHeight="1">
-      <c r="B47" s="11"/>
+      <c r="B47" s="11" t="s">
+        <v>316</v>
+      </c>
       <c r="AA47" s="5" t="s">
         <v>316</v>
       </c>
@@ -5580,9 +5833,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD63"/>
+  <dimension ref="A1:AH63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5651,7 +5906,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="178" customHeight="1">
+    <row r="11" spans="1:30" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:30" ht="24" customHeight="1">
@@ -5721,7 +5976,9 @@
       </c>
     </row>
     <row r="23" spans="1:34" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>347</v>
+      </c>
       <c r="AA23" s="5" t="s">
         <v>342</v>
       </c>
@@ -5767,7 +6024,9 @@
       </c>
     </row>
     <row r="27" spans="1:34" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11">
+        <v>72000</v>
+      </c>
     </row>
     <row r="30" spans="1:34" ht="24" customHeight="1">
       <c r="A30" s="12" t="s">
@@ -5833,7 +6092,9 @@
       </c>
     </row>
     <row r="39" spans="1:34" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>347</v>
+      </c>
       <c r="AA39" s="5" t="s">
         <v>342</v>
       </c>
@@ -5914,7 +6175,9 @@
       </c>
     </row>
     <row r="51" spans="1:30" ht="24" customHeight="1">
-      <c r="B51" s="11"/>
+      <c r="B51" s="11" t="s">
+        <v>333</v>
+      </c>
       <c r="AA51" s="5" t="s">
         <v>333</v>
       </c>
@@ -6018,9 +6281,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD80"/>
+  <dimension ref="A1:AE80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6089,7 +6354,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -6147,7 +6412,9 @@
       </c>
     </row>
     <row r="23" spans="1:28" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
+      <c r="B23" s="11" t="s">
+        <v>404</v>
+      </c>
       <c r="AA23" s="5" t="s">
         <v>404</v>
       </c>
@@ -6175,7 +6442,9 @@
       </c>
     </row>
     <row r="27" spans="1:28" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>863</v>
+      </c>
     </row>
     <row r="29" spans="1:28" ht="24" customHeight="1">
       <c r="A29" s="7" t="s">
@@ -6197,7 +6466,9 @@
       </c>
     </row>
     <row r="31" spans="1:28" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="24" customHeight="1">
       <c r="A34" s="12" t="s">
@@ -6463,7 +6734,9 @@
       </c>
     </row>
     <row r="80" spans="1:3" ht="24" customHeight="1">
-      <c r="B80" s="11"/>
+      <c r="B80" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="7">
@@ -6480,8 +6753,8 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
       <formula1>AA60:AE60</formula1>
@@ -6496,9 +6769,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD139"/>
+  <dimension ref="A1:AF139"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B128" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6567,7 +6842,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="178" customHeight="1">
+    <row r="11" spans="1:29" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
@@ -6669,7 +6944,9 @@
       </c>
     </row>
     <row r="31" spans="1:32" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>490</v>
+      </c>
       <c r="AA31" s="5" t="s">
         <v>486</v>
       </c>
@@ -6709,7 +6986,9 @@
       </c>
     </row>
     <row r="35" spans="1:30" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>495</v>
+      </c>
       <c r="AA35" s="5" t="s">
         <v>494</v>
       </c>
@@ -6740,7 +7019,9 @@
       </c>
     </row>
     <row r="39" spans="1:30" ht="24" customHeight="1">
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>500</v>
+      </c>
       <c r="AA39" s="5" t="s">
         <v>500</v>
       </c>
@@ -6787,7 +7068,9 @@
       </c>
     </row>
     <row r="47" spans="1:30" ht="24" customHeight="1">
-      <c r="B47" s="11"/>
+      <c r="B47" s="11" t="s">
+        <v>511</v>
+      </c>
       <c r="AA47" s="5" t="s">
         <v>509</v>
       </c>
@@ -6944,7 +7227,9 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+      <c r="B75" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="24" customHeight="1">
       <c r="A77" s="7" t="s">
@@ -6966,7 +7251,9 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="24" customHeight="1">
-      <c r="B79" s="11"/>
+      <c r="B79" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:32" ht="24" customHeight="1">
       <c r="A82" s="12" t="s">
@@ -7001,7 +7288,9 @@
       </c>
     </row>
     <row r="87" spans="1:32" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>488</v>
+      </c>
       <c r="AA87" s="5" t="s">
         <v>486</v>
       </c>
@@ -7041,7 +7330,9 @@
       </c>
     </row>
     <row r="91" spans="1:32" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
+      <c r="B91" s="11" t="s">
+        <v>494</v>
+      </c>
       <c r="AA91" s="5" t="s">
         <v>494</v>
       </c>
@@ -7072,7 +7363,9 @@
       </c>
     </row>
     <row r="95" spans="1:32" ht="24" customHeight="1">
-      <c r="B95" s="11"/>
+      <c r="B95" s="11" t="s">
+        <v>500</v>
+      </c>
       <c r="AA95" s="5" t="s">
         <v>500</v>
       </c>
@@ -7119,7 +7412,9 @@
       </c>
     </row>
     <row r="103" spans="1:30" ht="24" customHeight="1">
-      <c r="B103" s="11"/>
+      <c r="B103" s="11" t="s">
+        <v>509</v>
+      </c>
       <c r="AA103" s="5" t="s">
         <v>509</v>
       </c>
@@ -7153,7 +7448,9 @@
       </c>
     </row>
     <row r="107" spans="1:30" ht="24" customHeight="1">
-      <c r="B107" s="11"/>
+      <c r="B107" s="11">
+        <v>600</v>
+      </c>
     </row>
     <row r="109" spans="1:30" ht="24" customHeight="1">
       <c r="A109" s="7" t="s">
@@ -7197,7 +7494,9 @@
       </c>
     </row>
     <row r="115" spans="1:28" ht="24" customHeight="1">
-      <c r="B115" s="11"/>
+      <c r="B115" s="11">
+        <v>600</v>
+      </c>
     </row>
     <row r="117" spans="1:28" ht="24" customHeight="1">
       <c r="A117" s="7" t="s">
@@ -7254,7 +7553,9 @@
       </c>
     </row>
     <row r="127" spans="1:28" ht="24" customHeight="1">
-      <c r="B127" s="11"/>
+      <c r="B127" s="11" t="s">
+        <v>578</v>
+      </c>
       <c r="AA127" s="5" t="s">
         <v>578</v>
       </c>
@@ -7304,7 +7605,9 @@
       </c>
     </row>
     <row r="135" spans="1:3" ht="24" customHeight="1">
-      <c r="B135" s="11"/>
+      <c r="B135" s="11" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="7" t="s">
@@ -7326,7 +7629,9 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
-      <c r="B139" s="11"/>
+      <c r="B139" s="11" t="s">
+        <v>865</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="18">
@@ -7391,9 +7696,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD135"/>
+  <dimension ref="A1:AI135"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B127" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7462,7 +7769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -7568,7 +7875,9 @@
       </c>
     </row>
     <row r="35" spans="1:35" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="AA35" s="5" t="s">
         <v>619</v>
       </c>
@@ -7859,7 +8168,9 @@
       </c>
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
-      <c r="B83" s="11"/>
+      <c r="B83" s="11" t="s">
+        <v>667</v>
+      </c>
       <c r="AA83" s="5" t="s">
         <v>666</v>
       </c>
@@ -7893,7 +8204,9 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>866</v>
+      </c>
     </row>
     <row r="89" spans="1:30" ht="24" customHeight="1">
       <c r="A89" s="7" t="s">
@@ -7915,7 +8228,9 @@
       </c>
     </row>
     <row r="91" spans="1:30" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
+      <c r="B91" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:30" ht="24" customHeight="1">
       <c r="A93" s="7" t="s">
@@ -7972,7 +8287,12 @@
       </c>
     </row>
     <row r="103" spans="1:33" ht="24" customHeight="1">
-      <c r="B103" s="11"/>
+      <c r="B103" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>867</v>
+      </c>
       <c r="AA103" s="5" t="s">
         <v>619</v>
       </c>
@@ -8015,7 +8335,9 @@
       </c>
     </row>
     <row r="107" spans="1:33" ht="24" customHeight="1">
-      <c r="B107" s="11"/>
+      <c r="B107" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="109" spans="1:33" ht="24" customHeight="1">
       <c r="A109" s="7" t="s">
@@ -8094,7 +8416,12 @@
       </c>
     </row>
     <row r="123" spans="1:33" ht="24" customHeight="1">
-      <c r="B123" s="11"/>
+      <c r="B123" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>868</v>
+      </c>
       <c r="AA123" s="5" t="s">
         <v>619</v>
       </c>
@@ -8192,8 +8519,8 @@
       <formula1>AA35:AI35</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
       <formula1>0</formula1>
@@ -8202,8 +8529,8 @@
       <formula1>AA55:AI55</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
       <formula1>0</formula1>
@@ -8239,9 +8566,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD45"/>
+  <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8310,7 +8639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -8431,7 +8760,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="178" customHeight="1">
+    <row r="32" spans="1:34" ht="177.95" customHeight="1">
       <c r="B32" s="11"/>
     </row>
     <row r="34" spans="1:29" ht="24" customHeight="1">
@@ -8454,7 +8783,9 @@
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1">
-      <c r="B36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>749</v>
+      </c>
       <c r="AA36" s="5" t="s">
         <v>749</v>
       </c>
@@ -8485,7 +8816,9 @@
       </c>
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1">
-      <c r="B40" s="11"/>
+      <c r="B40" s="11">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" spans="1:29" ht="24" customHeight="1">
       <c r="A42" s="7" t="s">
@@ -8511,7 +8844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="178" customHeight="1">
+    <row r="45" spans="1:29" ht="177.95" customHeight="1">
       <c r="B45" s="11"/>
     </row>
   </sheetData>

</xml_diff>